<commit_message>
Obtained number of ensembl genes for each GO term in supplementary file.
</commit_message>
<xml_diff>
--- a/data/Supplementary_Table_9_ng_3259_S10.xlsx
+++ b/data/Supplementary_Table_9_ng_3259_S10.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicochaves/Dropbox/Stanford/CS341_Code/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicochaves/Documents/Stanford/CS341_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9904" uniqueCount="6623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9903" uniqueCount="6622">
   <si>
     <t>BTO:0003939</t>
   </si>
@@ -19901,9 +19901,6 @@
       </rPr>
       <t>: We used simple text mining followed by manual curation to map biological process (BP) terms in GO to tissue terms in the BRENDA Tissue ontology. This table provides the constructed mappings.</t>
     </r>
-  </si>
-  <si>
-    <t>(ovary??)</t>
   </si>
 </sst>
 </file>
@@ -20317,7 +20314,7 @@
   <dimension ref="A1:AEC225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B221" sqref="B221"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20348,9 +20345,6 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>6622</v>
-      </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" t="s">

</xml_diff>